<commit_message>
lot of fixes, reruns etc.
</commit_message>
<xml_diff>
--- a/data/99. analyzes/excel/pharmas/anzahl_empfaenger.xlsx
+++ b/data/99. analyzes/excel/pharmas/anzahl_empfaenger.xlsx
@@ -182,10 +182,10 @@
     <t>allergan</t>
   </si>
   <si>
+    <t>theramex</t>
+  </si>
+  <si>
     <t>gruenenthal</t>
-  </si>
-  <si>
-    <t>theramex</t>
   </si>
   <si>
     <t>nordic</t>
@@ -613,10 +613,10 @@
         <v>416</v>
       </c>
       <c r="D4" t="n">
-        <v>16717423</v>
+        <v>16715103</v>
       </c>
       <c r="E4" t="n">
-        <v>40186</v>
+        <v>40181</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -715,10 +715,10 @@
         <v>173</v>
       </c>
       <c r="D10" t="n">
-        <v>4537535</v>
+        <v>4537484</v>
       </c>
       <c r="E10" t="n">
-        <v>26229</v>
+        <v>26228</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -817,7 +817,7 @@
         <v>206</v>
       </c>
       <c r="D16" t="n">
-        <v>3119493.92</v>
+        <v>3119493.91</v>
       </c>
       <c r="E16" t="n">
         <v>15143</v>
@@ -834,7 +834,7 @@
         <v>844</v>
       </c>
       <c r="D17" t="n">
-        <v>11915637.6</v>
+        <v>11915637.61</v>
       </c>
       <c r="E17" t="n">
         <v>14118</v>
@@ -919,7 +919,7 @@
         <v>39</v>
       </c>
       <c r="D22" t="n">
-        <v>386943.47</v>
+        <v>386943.46</v>
       </c>
       <c r="E22" t="n">
         <v>9922</v>
@@ -953,7 +953,7 @@
         <v>262</v>
       </c>
       <c r="D24" t="n">
-        <v>2467588</v>
+        <v>2467592</v>
       </c>
       <c r="E24" t="n">
         <v>9418</v>
@@ -987,7 +987,7 @@
         <v>408</v>
       </c>
       <c r="D26" t="n">
-        <v>3759699</v>
+        <v>3759699.3</v>
       </c>
       <c r="E26" t="n">
         <v>9215</v>
@@ -1072,7 +1072,7 @@
         <v>180</v>
       </c>
       <c r="D31" t="n">
-        <v>1317573.68</v>
+        <v>1317573.67</v>
       </c>
       <c r="E31" t="n">
         <v>7320</v>
@@ -1089,7 +1089,7 @@
         <v>359</v>
       </c>
       <c r="D32" t="n">
-        <v>2517369.9</v>
+        <v>2517371.2</v>
       </c>
       <c r="E32" t="n">
         <v>7012</v>
@@ -1123,10 +1123,10 @@
         <v>338</v>
       </c>
       <c r="D34" t="n">
-        <v>1784313.55</v>
+        <v>1785331.25</v>
       </c>
       <c r="E34" t="n">
-        <v>5279</v>
+        <v>5282</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1225,7 +1225,7 @@
         <v>58</v>
       </c>
       <c r="D40" t="n">
-        <v>216390</v>
+        <v>216392</v>
       </c>
       <c r="E40" t="n">
         <v>3731</v>
@@ -1395,7 +1395,7 @@
         <v>62</v>
       </c>
       <c r="D50" t="n">
-        <v>173693.9</v>
+        <v>173693.91</v>
       </c>
       <c r="E50" t="n">
         <v>2802</v>
@@ -1437,36 +1437,36 @@
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="1" t="n">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
         <v>55</v>
       </c>
       <c r="C53" t="n">
-        <v>153</v>
+        <v>26</v>
       </c>
       <c r="D53" t="n">
-        <v>330000</v>
+        <v>61065</v>
       </c>
       <c r="E53" t="n">
-        <v>2157</v>
+        <v>2349</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="1" t="n">
-        <v>53</v>
+        <v>23</v>
       </c>
       <c r="B54" t="s">
         <v>56</v>
       </c>
       <c r="C54" t="n">
-        <v>26</v>
+        <v>153</v>
       </c>
       <c r="D54" t="n">
-        <v>48639</v>
+        <v>329993</v>
       </c>
       <c r="E54" t="n">
-        <v>1871</v>
+        <v>2157</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1497,10 +1497,10 @@
         <v>83</v>
       </c>
       <c r="D56" t="n">
-        <v>118602.02</v>
+        <v>118542.02</v>
       </c>
       <c r="E56" t="n">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="57" spans="1:5">

</xml_diff>

<commit_message>
fix acc in list
</commit_message>
<xml_diff>
--- a/data/99. analyzes/excel/pharmas/anzahl_empfaenger.xlsx
+++ b/data/99. analyzes/excel/pharmas/anzahl_empfaenger.xlsx
@@ -642,7 +642,7 @@
         <v>114</v>
       </c>
       <c r="E4" t="n">
-        <v>1388257</v>
+        <v>1546494.75</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -663,7 +663,7 @@
         <v>222</v>
       </c>
       <c r="E5" t="n">
-        <v>229002</v>
+        <v>238836.5</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
@@ -726,11 +726,11 @@
         <v>28</v>
       </c>
       <c r="E8" t="n">
-        <v>81133</v>
+        <v>83353</v>
       </c>
       <c r="F8" t="s"/>
       <c r="G8" t="n">
-        <v>2898</v>
+        <v>2977</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -747,11 +747,11 @@
         <v>100</v>
       </c>
       <c r="E9" t="n">
-        <v>215893</v>
+        <v>231991</v>
       </c>
       <c r="F9" t="s"/>
       <c r="G9" t="n">
-        <v>2159</v>
+        <v>2320</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -768,11 +768,11 @@
         <v>61</v>
       </c>
       <c r="E10" t="n">
-        <v>480567.8900000001</v>
+        <v>522803.4600000001</v>
       </c>
       <c r="F10" t="s"/>
       <c r="G10" t="n">
-        <v>7878</v>
+        <v>8571</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -789,11 +789,11 @@
         <v>85</v>
       </c>
       <c r="E11" t="n">
-        <v>52041.85000000001</v>
+        <v>96216.29000000001</v>
       </c>
       <c r="F11" t="s"/>
       <c r="G11" t="n">
-        <v>612</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -810,11 +810,11 @@
         <v>134</v>
       </c>
       <c r="E12" t="n">
-        <v>5544084.809999997</v>
+        <v>5671473.469999997</v>
       </c>
       <c r="F12" t="s"/>
       <c r="G12" t="n">
-        <v>41374</v>
+        <v>42324</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -831,11 +831,11 @@
         <v>244</v>
       </c>
       <c r="E13" t="n">
-        <v>303259.1600000001</v>
+        <v>457701.6200000001</v>
       </c>
       <c r="F13" t="s"/>
       <c r="G13" t="n">
-        <v>1243</v>
+        <v>1876</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -852,11 +852,11 @@
         <v>60</v>
       </c>
       <c r="E14" t="n">
-        <v>775673.2500000002</v>
+        <v>974545.1100000002</v>
       </c>
       <c r="F14" t="s"/>
       <c r="G14" t="n">
-        <v>12928</v>
+        <v>16242</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -873,11 +873,11 @@
         <v>56</v>
       </c>
       <c r="E15" t="n">
-        <v>81851.42999999998</v>
+        <v>120264.34</v>
       </c>
       <c r="F15" t="s"/>
       <c r="G15" t="n">
-        <v>1462</v>
+        <v>2148</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -915,11 +915,11 @@
         <v>206</v>
       </c>
       <c r="E17" t="n">
-        <v>388005.1800000001</v>
+        <v>423709.1800000001</v>
       </c>
       <c r="F17" t="s"/>
       <c r="G17" t="n">
-        <v>1884</v>
+        <v>2057</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -978,11 +978,11 @@
         <v>228</v>
       </c>
       <c r="E20" t="n">
-        <v>6141480.390000001</v>
+        <v>6142680.390000001</v>
       </c>
       <c r="F20" t="s"/>
       <c r="G20" t="n">
-        <v>26936</v>
+        <v>26942</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -999,11 +999,11 @@
         <v>614</v>
       </c>
       <c r="E21" t="n">
-        <v>947440.62</v>
+        <v>992283.65</v>
       </c>
       <c r="F21" t="s"/>
       <c r="G21" t="n">
-        <v>1543</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1104,11 +1104,11 @@
         <v>96</v>
       </c>
       <c r="E26" t="n">
-        <v>4663670.379999999</v>
+        <v>4672970.379999999</v>
       </c>
       <c r="F26" t="s"/>
       <c r="G26" t="n">
-        <v>48580</v>
+        <v>48677</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1125,11 +1125,11 @@
         <v>243</v>
       </c>
       <c r="E27" t="n">
-        <v>197013.6200000001</v>
+        <v>306345.9</v>
       </c>
       <c r="F27" t="s"/>
       <c r="G27" t="n">
-        <v>811</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1146,11 +1146,11 @@
         <v>122</v>
       </c>
       <c r="E28" t="n">
-        <v>4347209.029999999</v>
+        <v>4350106.529999999</v>
       </c>
       <c r="F28" t="s"/>
       <c r="G28" t="n">
-        <v>35633</v>
+        <v>35657</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1167,11 +1167,11 @@
         <v>81</v>
       </c>
       <c r="E29" t="n">
-        <v>183704.33</v>
+        <v>227889.38</v>
       </c>
       <c r="F29" t="s"/>
       <c r="G29" t="n">
-        <v>2268</v>
+        <v>2813</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1209,11 +1209,11 @@
         <v>14</v>
       </c>
       <c r="E31" t="n">
-        <v>33409.8</v>
+        <v>34405.8</v>
       </c>
       <c r="F31" t="s"/>
       <c r="G31" t="n">
-        <v>2386</v>
+        <v>2458</v>
       </c>
     </row>
     <row r="32" spans="1:7">
@@ -1251,11 +1251,11 @@
         <v>291</v>
       </c>
       <c r="E33" t="n">
-        <v>399291.67</v>
+        <v>495998.16</v>
       </c>
       <c r="F33" t="s"/>
       <c r="G33" t="n">
-        <v>1372</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="34" spans="1:7">
@@ -1272,7 +1272,7 @@
         <v>62</v>
       </c>
       <c r="E34" t="n">
-        <v>515945</v>
+        <v>523945</v>
       </c>
       <c r="F34" t="b">
         <v>1</v>
@@ -1293,7 +1293,7 @@
         <v>53</v>
       </c>
       <c r="E35" t="n">
-        <v>75147.89</v>
+        <v>164255</v>
       </c>
       <c r="F35" t="b">
         <v>1</v>
@@ -1356,7 +1356,7 @@
         <v>109</v>
       </c>
       <c r="E38" t="n">
-        <v>2122876</v>
+        <v>2163235</v>
       </c>
       <c r="F38" t="b">
         <v>1</v>
@@ -1377,7 +1377,7 @@
         <v>175</v>
       </c>
       <c r="E39" t="n">
-        <v>208155</v>
+        <v>297076</v>
       </c>
       <c r="F39" t="b">
         <v>1</v>
@@ -1398,11 +1398,11 @@
         <v>29</v>
       </c>
       <c r="E40" t="n">
-        <v>159099</v>
+        <v>168867</v>
       </c>
       <c r="F40" t="s"/>
       <c r="G40" t="n">
-        <v>5486</v>
+        <v>5823</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -1419,11 +1419,11 @@
         <v>28</v>
       </c>
       <c r="E41" t="n">
-        <v>44201</v>
+        <v>47525</v>
       </c>
       <c r="F41" t="s"/>
       <c r="G41" t="n">
-        <v>1579</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -1499,11 +1499,11 @@
         <v>25</v>
       </c>
       <c r="E45" t="n">
-        <v>48486.8</v>
+        <v>198169.85</v>
       </c>
       <c r="F45" t="s"/>
       <c r="G45" t="n">
-        <v>1939</v>
+        <v>7927</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -1541,11 +1541,11 @@
         <v>87</v>
       </c>
       <c r="E47" t="n">
-        <v>127149</v>
+        <v>128524</v>
       </c>
       <c r="F47" t="s"/>
       <c r="G47" t="n">
-        <v>1461</v>
+        <v>1477</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -1562,11 +1562,11 @@
         <v>129</v>
       </c>
       <c r="E48" t="n">
-        <v>4028981.33</v>
+        <v>4031381.33</v>
       </c>
       <c r="F48" t="s"/>
       <c r="G48" t="n">
-        <v>31232</v>
+        <v>31251</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -1625,11 +1625,11 @@
         <v>95</v>
       </c>
       <c r="E51" t="n">
-        <v>41914</v>
+        <v>71110</v>
       </c>
       <c r="F51" t="s"/>
       <c r="G51" t="n">
-        <v>441</v>
+        <v>749</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -1646,11 +1646,11 @@
         <v>2</v>
       </c>
       <c r="E52" t="n">
-        <v>10770</v>
+        <v>11070</v>
       </c>
       <c r="F52" t="s"/>
       <c r="G52" t="n">
-        <v>5385</v>
+        <v>5535</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -1667,11 +1667,11 @@
         <v>1</v>
       </c>
       <c r="E53" t="n">
-        <v>0</v>
+        <v>251.83</v>
       </c>
       <c r="F53" t="s"/>
       <c r="G53" t="n">
-        <v>0</v>
+        <v>252</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -1688,11 +1688,11 @@
         <v>10</v>
       </c>
       <c r="E54" t="n">
-        <v>0</v>
+        <v>198085.28</v>
       </c>
       <c r="F54" t="s"/>
       <c r="G54" t="n">
-        <v>0</v>
+        <v>19809</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -1709,11 +1709,11 @@
         <v>27</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>45091.76</v>
       </c>
       <c r="F55" t="s"/>
       <c r="G55" t="n">
-        <v>0</v>
+        <v>1670</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -1730,11 +1730,11 @@
         <v>136</v>
       </c>
       <c r="E56" t="n">
-        <v>2198030</v>
+        <v>2475216</v>
       </c>
       <c r="F56" t="s"/>
       <c r="G56" t="n">
-        <v>16162</v>
+        <v>18200</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -1751,11 +1751,11 @@
         <v>463</v>
       </c>
       <c r="E57" t="n">
-        <v>357812</v>
+        <v>682064</v>
       </c>
       <c r="F57" t="s"/>
       <c r="G57" t="n">
-        <v>773</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -1856,11 +1856,11 @@
         <v>176</v>
       </c>
       <c r="E62" t="n">
-        <v>5738751.62</v>
+        <v>6088291.05</v>
       </c>
       <c r="F62" t="s"/>
       <c r="G62" t="n">
-        <v>32607</v>
+        <v>34593</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -1877,11 +1877,11 @@
         <v>208</v>
       </c>
       <c r="E63" t="n">
-        <v>500161.6500000001</v>
+        <v>549989.6200000001</v>
       </c>
       <c r="F63" t="s"/>
       <c r="G63" t="n">
-        <v>2405</v>
+        <v>2644</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -1898,11 +1898,11 @@
         <v>53</v>
       </c>
       <c r="E64" t="n">
-        <v>242439</v>
+        <v>252959</v>
       </c>
       <c r="F64" t="s"/>
       <c r="G64" t="n">
-        <v>4574</v>
+        <v>4773</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -1940,11 +1940,11 @@
         <v>146</v>
       </c>
       <c r="E66" t="n">
-        <v>755861</v>
+        <v>762861</v>
       </c>
       <c r="F66" t="s"/>
       <c r="G66" t="n">
-        <v>5177</v>
+        <v>5225</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -2003,11 +2003,11 @@
         <v>171</v>
       </c>
       <c r="E69" t="n">
-        <v>250685.3099999999</v>
+        <v>301744.1599999999</v>
       </c>
       <c r="F69" t="s"/>
       <c r="G69" t="n">
-        <v>1466</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -2045,11 +2045,11 @@
         <v>23</v>
       </c>
       <c r="E71" t="n">
-        <v>37229.4</v>
+        <v>45229.4</v>
       </c>
       <c r="F71" t="s"/>
       <c r="G71" t="n">
-        <v>1619</v>
+        <v>1966</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -2108,11 +2108,11 @@
         <v>55</v>
       </c>
       <c r="E74" t="n">
-        <v>179772</v>
+        <v>198272</v>
       </c>
       <c r="F74" t="s"/>
       <c r="G74" t="n">
-        <v>3269</v>
+        <v>3605</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -2129,11 +2129,11 @@
         <v>26</v>
       </c>
       <c r="E75" t="n">
-        <v>22451</v>
+        <v>35439</v>
       </c>
       <c r="F75" t="s"/>
       <c r="G75" t="n">
-        <v>864</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -2190,11 +2190,11 @@
         <v>21</v>
       </c>
       <c r="E78" t="n">
-        <v>26000</v>
+        <v>64467.85</v>
       </c>
       <c r="F78" t="s"/>
       <c r="G78" t="n">
-        <v>1238</v>
+        <v>3070</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -2211,11 +2211,11 @@
         <v>6</v>
       </c>
       <c r="E79" t="n">
-        <v>7120</v>
+        <v>13810</v>
       </c>
       <c r="F79" t="s"/>
       <c r="G79" t="n">
-        <v>1187</v>
+        <v>2302</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -2232,7 +2232,7 @@
         <v>270</v>
       </c>
       <c r="E80" t="n">
-        <v>12969995.7</v>
+        <v>13069251.35</v>
       </c>
       <c r="F80" t="b">
         <v>1</v>
@@ -2253,7 +2253,7 @@
         <v>448</v>
       </c>
       <c r="E81" t="n">
-        <v>595710.6799999998</v>
+        <v>595715.6799999998</v>
       </c>
       <c r="F81" t="b">
         <v>1</v>
@@ -2274,11 +2274,11 @@
         <v>108</v>
       </c>
       <c r="E82" t="n">
-        <v>1795912</v>
+        <v>2097912</v>
       </c>
       <c r="F82" t="s"/>
       <c r="G82" t="n">
-        <v>16629</v>
+        <v>19425</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -2295,11 +2295,11 @@
         <v>299</v>
       </c>
       <c r="E83" t="n">
-        <v>417631.3</v>
+        <v>549679.3</v>
       </c>
       <c r="F83" t="s"/>
       <c r="G83" t="n">
-        <v>1397</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -2337,11 +2337,11 @@
         <v>30</v>
       </c>
       <c r="E85" t="n">
-        <v>23998.86</v>
+        <v>28533.13</v>
       </c>
       <c r="F85" t="s"/>
       <c r="G85" t="n">
-        <v>800</v>
+        <v>951</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -2379,7 +2379,7 @@
         <v>25</v>
       </c>
       <c r="E87" t="n">
-        <v>30614.73</v>
+        <v>44348.27</v>
       </c>
       <c r="F87" t="b">
         <v>1</v>
@@ -2400,11 +2400,11 @@
         <v>241</v>
       </c>
       <c r="E88" t="n">
-        <v>8592463</v>
+        <v>8595051</v>
       </c>
       <c r="F88" t="s"/>
       <c r="G88" t="n">
-        <v>35653</v>
+        <v>35664</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -2421,11 +2421,11 @@
         <v>173</v>
       </c>
       <c r="E89" t="n">
-        <v>294322</v>
+        <v>324358</v>
       </c>
       <c r="F89" t="s"/>
       <c r="G89" t="n">
-        <v>1701</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -2442,11 +2442,11 @@
         <v>64</v>
       </c>
       <c r="E90" t="n">
-        <v>215811.56</v>
+        <v>230827.26</v>
       </c>
       <c r="F90" t="s"/>
       <c r="G90" t="n">
-        <v>3372</v>
+        <v>3607</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -2463,11 +2463,11 @@
         <v>54</v>
       </c>
       <c r="E91" t="n">
-        <v>65270.38000000001</v>
+        <v>117359.72</v>
       </c>
       <c r="F91" t="s"/>
       <c r="G91" t="n">
-        <v>1209</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -2589,7 +2589,7 @@
         <v>45</v>
       </c>
       <c r="E97" t="n">
-        <v>46651.83</v>
+        <v>52925.44</v>
       </c>
       <c r="F97" t="b">
         <v>1</v>
@@ -2610,7 +2610,7 @@
         <v>54</v>
       </c>
       <c r="E98" t="n">
-        <v>478555.72</v>
+        <v>2273127.68</v>
       </c>
       <c r="F98" t="b">
         <v>1</v>
@@ -2631,7 +2631,7 @@
         <v>147</v>
       </c>
       <c r="E99" t="n">
-        <v>229227.12</v>
+        <v>592483.6599999999</v>
       </c>
       <c r="F99" t="b">
         <v>1</v>
@@ -2652,7 +2652,7 @@
         <v>118</v>
       </c>
       <c r="E100" t="n">
-        <v>2143708</v>
+        <v>2257443</v>
       </c>
       <c r="F100" t="b">
         <v>1</v>
@@ -2673,7 +2673,7 @@
         <v>138</v>
       </c>
       <c r="E101" t="n">
-        <v>146173</v>
+        <v>174598</v>
       </c>
       <c r="F101" t="b">
         <v>1</v>
@@ -2715,7 +2715,7 @@
         <v>19</v>
       </c>
       <c r="E103" t="n">
-        <v>35915.64</v>
+        <v>51335.92</v>
       </c>
       <c r="F103" t="b">
         <v>1</v>
@@ -2757,11 +2757,11 @@
         <v>22</v>
       </c>
       <c r="E105" t="n">
-        <v>31433.39</v>
+        <v>32722.16</v>
       </c>
       <c r="F105" t="s"/>
       <c r="G105" t="n">
-        <v>1429</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -2778,11 +2778,11 @@
         <v>88</v>
       </c>
       <c r="E106" t="n">
-        <v>1033444.22</v>
+        <v>1039194.22</v>
       </c>
       <c r="F106" t="s"/>
       <c r="G106" t="n">
-        <v>11744</v>
+        <v>11809</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -2799,11 +2799,11 @@
         <v>73</v>
       </c>
       <c r="E107" t="n">
-        <v>112131.19</v>
+        <v>151761.89</v>
       </c>
       <c r="F107" t="s"/>
       <c r="G107" t="n">
-        <v>1536</v>
+        <v>2079</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -2862,11 +2862,11 @@
         <v>49</v>
       </c>
       <c r="E110" t="n">
-        <v>2380691.89</v>
+        <v>2406646.04</v>
       </c>
       <c r="F110" t="s"/>
       <c r="G110" t="n">
-        <v>48586</v>
+        <v>49115</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -2883,11 +2883,11 @@
         <v>74</v>
       </c>
       <c r="E111" t="n">
-        <v>75474.88</v>
+        <v>96112.62000000001</v>
       </c>
       <c r="F111" t="s"/>
       <c r="G111" t="n">
-        <v>1020</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -2904,11 +2904,11 @@
         <v>238</v>
       </c>
       <c r="E112" t="n">
-        <v>2454155.5</v>
+        <v>2486008.200000001</v>
       </c>
       <c r="F112" t="s"/>
       <c r="G112" t="n">
-        <v>10312</v>
+        <v>10445</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -2925,11 +2925,11 @@
         <v>481</v>
       </c>
       <c r="E113" t="n">
-        <v>559983.2999999998</v>
+        <v>632524.8299999998</v>
       </c>
       <c r="F113" t="s"/>
       <c r="G113" t="n">
-        <v>1164</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="114" spans="1:7">

</xml_diff>